<commit_message>
back to caps on column headers
</commit_message>
<xml_diff>
--- a/etc/centers.xlsx
+++ b/etc/centers.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10095"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="centers" sheetId="1" r:id="rId1"/>
     <sheet name="ESRI_MAPINFO_SHEET" sheetId="2" state="veryHidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -1015,13 +1015,13 @@
     <t>BLDG_ADD</t>
   </si>
   <si>
-    <t>Borocode</t>
-  </si>
-  <si>
     <t>ZIP_CODE</t>
   </si>
   <si>
-    <t>Accessible</t>
+    <t>BOROCODE</t>
+  </si>
+  <si>
+    <t>ACCESSIBLE</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1498,7 @@
         <v>330</v>
       </c>
       <c r="F1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -1510,7 +1510,7 @@
         <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K1" t="s">
         <v>333</v>

</xml_diff>